<commit_message>
loading in full final dataset, preprocessing/data cleaning, save climate
</commit_message>
<xml_diff>
--- a/Data/Flowering_WVPT_life_history.xlsx
+++ b/Data/Flowering_WVPT_life_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avawessel/Desktop/Thesis_25/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FE983C-7BFE-4945-A8F9-6023B77101B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2DF609-6409-DD4F-8A75-6E274E07B78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16040" xr2:uid="{2E69A51F-874F-D441-893E-0D84F8DA87C5}"/>
+    <workbookView xWindow="10300" yWindow="500" windowWidth="18120" windowHeight="16040" xr2:uid="{2E69A51F-874F-D441-893E-0D84F8DA87C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Plectritis congesta</t>
   </si>
   <si>
-    <t>Lupinus polycarpus</t>
-  </si>
-  <si>
     <t>Collinsia grandiflora</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Tellima grandiflora</t>
+  </si>
+  <si>
+    <t>Lupinus bicolor</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
@@ -677,79 +677,79 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>3</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>3</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>3</v>
@@ -781,10 +781,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>